<commit_message>
Aggiunta storia, stanze, mappa, oggetti, nuovi comandi
</commit_message>
<xml_diff>
--- a/Mappa.xlsx
+++ b/Mappa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desktop\progetto\map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mstel\Corona-Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21ECEC5D-A15F-4C0F-89BD-84ECB171066E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAE4892-496F-4795-B1AF-DBAD7455BF5D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3150" yWindow="570" windowWidth="17340" windowHeight="7875" xr2:uid="{DC705764-6BB6-47B2-A905-C3F27DB4EA51}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875" xr2:uid="{DC705764-6BB6-47B2-A905-C3F27DB4EA51}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -32,22 +32,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>PASSAGGIO 
 SEGRETO</t>
   </si>
   <si>
-    <t>CORRIDOIO</t>
-  </si>
-  <si>
     <t>SCALE</t>
   </si>
   <si>
-    <t>FINE 
-CORRIDOIO</t>
-  </si>
-  <si>
     <t>CELLA 16</t>
   </si>
   <si>
@@ -64,9 +57,6 @@
   </si>
   <si>
     <t>CELLA 19</t>
-  </si>
-  <si>
-    <t>MURO</t>
   </si>
   <si>
     <t>ATRIO</t>
@@ -92,12 +82,6 @@
     <t>PALESTRA</t>
   </si>
   <si>
-    <t>ISOLAMENTO</t>
-  </si>
-  <si>
-    <t>PORTA USCITA BRACCIO</t>
-  </si>
-  <si>
     <t>ATRIO
 ISOLAMENTO</t>
   </si>
@@ -106,9 +90,6 @@
 FRATELLO</t>
   </si>
   <si>
-    <t>GRATA CELLA</t>
-  </si>
-  <si>
     <t>SCALA</t>
   </si>
   <si>
@@ -162,6 +143,57 @@
   <si>
     <t>secondo 
 piano</t>
+  </si>
+  <si>
+    <t>CORRIDOIO
+NORD</t>
+  </si>
+  <si>
+    <t>CORRIDOIO
+EST</t>
+  </si>
+  <si>
+    <t>CORRIDOIO
+SUD</t>
+  </si>
+  <si>
+    <t>FINE
+ATRIO</t>
+  </si>
+  <si>
+    <t>SUD
+ATRIO</t>
+  </si>
+  <si>
+    <t>CONDTTO
+EST CON
+GRATA CELLA</t>
+  </si>
+  <si>
+    <t>MURO
+(non descritto)</t>
+  </si>
+  <si>
+    <t>FINE 
+CORRIDOIO
+(non descritto)</t>
+  </si>
+  <si>
+    <t>PORTA USCITA BRACCIO
+(non descritto)</t>
+  </si>
+  <si>
+    <t>MURO
+ESTERNO
+ PRIGIONE</t>
+  </si>
+  <si>
+    <t>FUORI
+ISOLAMENTO</t>
+  </si>
+  <si>
+    <t>PORTA
+ISOLAMENTO</t>
   </si>
 </sst>
 </file>
@@ -254,21 +286,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="mediumDashed">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="mediumDashed">
-        <color auto="1"/>
-      </top>
-      <bottom style="mediumDashed">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color auto="1"/>
       </left>
@@ -544,11 +561,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="mediumDashed">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="mediumDashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -562,94 +592,103 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -967,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6875FA53-81C7-4357-B5EB-0C0145F43673}">
   <dimension ref="D1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="79" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,10 +1015,10 @@
     <col min="3" max="3" width="2.140625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
@@ -989,201 +1028,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:12" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="D1" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="4:12" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="22"/>
-      <c r="E2" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>27</v>
+      <c r="D2" s="18"/>
+      <c r="E2" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="4:12" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="22"/>
-      <c r="E3" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="22"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="4:12" ht="47.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="19" t="s">
+      <c r="D4" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="E4" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="G4" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
     </row>
     <row r="5" spans="4:12" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="29"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="1" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="29"/>
+      <c r="J5" s="12" t="s">
         <v>10</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="16" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="4:12" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="30"/>
-      <c r="E6" s="27"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="26"/>
       <c r="F6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="J6" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="37" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="4:12" ht="51" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="30"/>
-      <c r="E7" s="28"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="27"/>
       <c r="F7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="13" t="s">
         <v>11</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="4:12" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="13" t="s">
-        <v>25</v>
+      <c r="E8" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="19" t="s">
-        <v>17</v>
+        <v>26</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="4:12" ht="49.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>16</v>
+      <c r="F9" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="33" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="4:12" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="12" t="s">
-        <v>23</v>
+      <c r="E10" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" s="19" t="s">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="34" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="4:12" ht="51" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E11" s="23" t="s">
-        <v>24</v>
+      <c r="E11" s="19" t="s">
+        <v>18</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="22"/>
-      <c r="K11" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L11" s="20" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="18"/>
+      <c r="K11" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="4:12" ht="48" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
+      <c r="E12" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
     </row>
     <row r="15" spans="4:12" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="4:12" ht="47.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>